<commit_message>
Profesiograms ready for Andy 🥳
</commit_message>
<xml_diff>
--- a/AnalisisDeEntrada/DATA_FINAL.xlsx
+++ b/AnalisisDeEntrada/DATA_FINAL.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlospenaloza/Universidad/Simulación/SimulationProject/AnalisisDeEntrada/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasacevedo/Desktop/SimulationProject/AnalisisDeEntrada/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28CE927-FBCD-B74D-BED4-FFB96DA2481E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B79BF9E-014A-4E4A-8141-F7A471340A00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
     <sheet name="Toma1y2" sheetId="2" r:id="rId2"/>
     <sheet name="Toma3y4" sheetId="3" r:id="rId3"/>
+    <sheet name="Profesiogramas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="51">
   <si>
     <t>Recepción2</t>
   </si>
@@ -103,15 +104,97 @@
   <si>
     <t>Weibull</t>
   </si>
+  <si>
+    <t>Médico</t>
+  </si>
+  <si>
+    <t>Enfermera</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Solo médico</t>
+  </si>
+  <si>
+    <t>Médico, laboratorio</t>
+  </si>
+  <si>
+    <t>Médico, laboratorio,optometría, audiometría</t>
+  </si>
+  <si>
+    <t>Médico, audiometría, optometría y espirometría</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profesiograma </t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>Médico con enfásis en Osteomuscular</t>
+  </si>
+  <si>
+    <t>Serología</t>
+  </si>
+  <si>
+    <t>Visiometría</t>
+  </si>
+  <si>
+    <t>Prueba de drogas</t>
+  </si>
+  <si>
+    <t>Vacuna antitetanica</t>
+  </si>
+  <si>
+    <t>RA test</t>
+  </si>
+  <si>
+    <t>Koh de uñas</t>
+  </si>
+  <si>
+    <t>Frotis de garganta</t>
+  </si>
+  <si>
+    <t>Corpológico</t>
+  </si>
+  <si>
+    <t>Certifación de alimentos</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Exámenes de los pacientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estaciones por las que pasa un paciente </t>
+  </si>
+  <si>
+    <t>Ruta a la que pertenece el paciente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="172" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +335,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -435,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -667,6 +756,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -712,7 +816,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -751,6 +855,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1074,13 +1195,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1192,7 +1313,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1236,7 +1357,7 @@
         <v>-0.42571720000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1280,7 +1401,7 @@
         <v>-0.42571720000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1330,7 +1451,7 @@
         <v>4.360474</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1380,7 +1501,7 @@
         <v>3.7475960000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1418,7 +1539,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1468,7 +1589,7 @@
         <v>0.98660530000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1518,7 +1639,7 @@
         <v>0.47770590000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1553,7 +1674,7 @@
         <v>2.72</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1588,7 +1709,7 @@
         <v>4.07</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1623,7 +1744,7 @@
         <v>4.22</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1658,7 +1779,7 @@
         <v>2.62</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1693,7 +1814,7 @@
         <v>3.17</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1728,7 +1849,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1763,7 +1884,7 @@
         <v>3.72</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1798,7 +1919,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1833,7 +1954,7 @@
         <v>2.4300000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1868,7 +1989,7 @@
         <v>3.18</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1903,7 +2024,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1938,7 +2059,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1973,7 +2094,7 @@
         <v>2.35</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2008,7 +2129,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2043,7 +2164,7 @@
         <v>4.13</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2078,7 +2199,7 @@
         <v>3.52</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2113,7 +2234,7 @@
         <v>3.73</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2148,7 +2269,7 @@
         <v>2.2799999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2183,7 +2304,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2218,7 +2339,7 @@
         <v>4.33</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2253,7 +2374,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2288,7 +2409,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2320,7 +2441,7 @@
       </c>
       <c r="I32" s="12"/>
     </row>
-    <row r="33" spans="1:9">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2352,7 +2473,7 @@
       </c>
       <c r="I33" s="12"/>
     </row>
-    <row r="34" spans="1:9">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2384,7 +2505,7 @@
       </c>
       <c r="I34" s="12"/>
     </row>
-    <row r="35" spans="1:9">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2416,7 +2537,7 @@
       </c>
       <c r="I35" s="12"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2443,7 +2564,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="37" spans="1:9">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2470,7 +2591,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2497,7 +2618,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2520,7 +2641,7 @@
         <v>1.97</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2543,7 +2664,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2566,7 +2687,7 @@
         <v>2.0699999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2589,7 +2710,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2612,7 +2733,7 @@
         <v>2.12</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2632,7 +2753,7 @@
         <v>3.95</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2648,7 +2769,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2657,7 +2778,7 @@
       </c>
       <c r="G46" s="20"/>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2666,7 +2787,7 @@
       </c>
       <c r="G47" s="20"/>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2675,7 +2796,7 @@
       </c>
       <c r="G48" s="20"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2684,7 +2805,7 @@
       </c>
       <c r="G49" s="20"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2705,12 +2826,12 @@
       <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>16</v>
       </c>
@@ -2755,7 +2876,7 @@
       <c r="X1" s="24"/>
       <c r="Y1" s="25"/>
     </row>
-    <row r="2" spans="1:27" ht="16" thickBot="1">
+    <row r="2" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="8" t="s">
         <v>18</v>
@@ -2830,7 +2951,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:27">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2909,7 +3030,7 @@
       <c r="Z3" s="17"/>
       <c r="AA3" s="17"/>
     </row>
-    <row r="4" spans="1:27">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2988,7 +3109,7 @@
       <c r="Z4" s="17"/>
       <c r="AA4" s="17"/>
     </row>
-    <row r="5" spans="1:27">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3067,7 +3188,7 @@
       <c r="Z5" s="17"/>
       <c r="AA5" s="17"/>
     </row>
-    <row r="6" spans="1:27">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3146,7 +3267,7 @@
       <c r="Z6" s="17"/>
       <c r="AA6" s="17"/>
     </row>
-    <row r="7" spans="1:27">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3225,7 +3346,7 @@
       <c r="Z7" s="17"/>
       <c r="AA7" s="17"/>
     </row>
-    <row r="8" spans="1:27">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3304,7 +3425,7 @@
       <c r="Z8" s="17"/>
       <c r="AA8" s="17"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3383,7 +3504,7 @@
       <c r="Z9" s="17"/>
       <c r="AA9" s="17"/>
     </row>
-    <row r="10" spans="1:27">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3462,7 +3583,7 @@
       <c r="Z10" s="17"/>
       <c r="AA10" s="17"/>
     </row>
-    <row r="11" spans="1:27">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3541,7 +3662,7 @@
       <c r="Z11" s="17"/>
       <c r="AA11" s="17"/>
     </row>
-    <row r="12" spans="1:27">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3620,7 +3741,7 @@
       <c r="Z12" s="17"/>
       <c r="AA12" s="17"/>
     </row>
-    <row r="13" spans="1:27">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3700,7 +3821,7 @@
       <c r="Z13" s="17"/>
       <c r="AA13" s="17"/>
     </row>
-    <row r="14" spans="1:27">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3780,7 +3901,7 @@
       <c r="Z14" s="17"/>
       <c r="AA14" s="17"/>
     </row>
-    <row r="15" spans="1:27">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3860,7 +3981,7 @@
       <c r="Z15" s="17"/>
       <c r="AA15" s="17"/>
     </row>
-    <row r="16" spans="1:27">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3940,7 +4061,7 @@
       <c r="Z16" s="17"/>
       <c r="AA16" s="17"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4012,7 +4133,7 @@
       <c r="X17" s="7"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4084,7 +4205,7 @@
       <c r="X18" s="4"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4155,7 +4276,7 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4226,7 +4347,7 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4291,7 +4412,7 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4344,7 +4465,7 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4397,7 +4518,7 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4444,7 +4565,7 @@
       <c r="X24" s="4"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4485,7 +4606,7 @@
       <c r="X25" s="4"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4520,7 +4641,7 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4555,7 +4676,7 @@
       <c r="X27" s="4"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4590,7 +4711,7 @@
       <c r="X28" s="4"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" spans="1:25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4625,7 +4746,7 @@
       <c r="X29" s="4"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4660,7 +4781,7 @@
       <c r="X30" s="4"/>
       <c r="Y30" s="5"/>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4695,7 +4816,7 @@
       <c r="X31" s="4"/>
       <c r="Y31" s="5"/>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -4730,7 +4851,7 @@
       <c r="X32" s="4"/>
       <c r="Y32" s="5"/>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4765,7 +4886,7 @@
       <c r="X33" s="4"/>
       <c r="Y33" s="5"/>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4800,7 +4921,7 @@
       <c r="X34" s="4"/>
       <c r="Y34" s="5"/>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4835,7 +4956,7 @@
       <c r="X35" s="4"/>
       <c r="Y35" s="5"/>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4870,7 +4991,7 @@
       <c r="X36" s="4"/>
       <c r="Y36" s="5"/>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7"/>
@@ -4897,7 +5018,7 @@
       <c r="X37" s="4"/>
       <c r="Y37" s="5"/>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="6"/>
       <c r="C38" s="7"/>
@@ -4924,7 +5045,7 @@
       <c r="X38" s="4"/>
       <c r="Y38" s="5"/>
     </row>
-    <row r="39" spans="1:25" ht="16" thickBot="1">
+    <row r="39" spans="1:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="8"/>
       <c r="C39" s="9"/>
@@ -4951,122 +5072,122 @@
       <c r="X39" s="9"/>
       <c r="Y39" s="10"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I41" s="15"/>
       <c r="R41" s="15"/>
       <c r="S41" s="16"/>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I42" s="15"/>
       <c r="R42" s="15"/>
       <c r="S42" s="16"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
       <c r="R43" s="15"/>
       <c r="S43" s="16"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I44" s="15"/>
       <c r="R44" s="15"/>
       <c r="S44" s="16"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I45" s="15"/>
       <c r="R45" s="15"/>
       <c r="S45" s="16"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="16"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I47" s="15"/>
       <c r="R47" s="15"/>
       <c r="S47" s="16"/>
     </row>
-    <row r="48" spans="1:25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.2">
       <c r="I48" s="15"/>
       <c r="R48" s="15"/>
       <c r="S48" s="16"/>
     </row>
-    <row r="49" spans="9:19">
+    <row r="49" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I49" s="15"/>
       <c r="R49" s="15"/>
       <c r="S49" s="16"/>
     </row>
-    <row r="50" spans="9:19">
+    <row r="50" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I50" s="15"/>
       <c r="R50" s="15"/>
       <c r="S50" s="16"/>
     </row>
-    <row r="51" spans="9:19">
+    <row r="51" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I51" s="15"/>
       <c r="R51" s="15"/>
       <c r="S51" s="16"/>
     </row>
-    <row r="52" spans="9:19">
+    <row r="52" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I52" s="15"/>
       <c r="R52" s="15"/>
       <c r="S52" s="16"/>
     </row>
-    <row r="53" spans="9:19">
+    <row r="53" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I53" s="15"/>
       <c r="R53" s="15"/>
       <c r="S53" s="16"/>
     </row>
-    <row r="54" spans="9:19">
+    <row r="54" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I54" s="15"/>
       <c r="R54" s="15"/>
       <c r="S54" s="16"/>
     </row>
-    <row r="55" spans="9:19">
+    <row r="55" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I55" s="15"/>
       <c r="R55" s="15"/>
       <c r="S55" s="16"/>
     </row>
-    <row r="56" spans="9:19">
+    <row r="56" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I56" s="15"/>
       <c r="R56" s="15"/>
       <c r="S56" s="16"/>
     </row>
-    <row r="57" spans="9:19">
+    <row r="57" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I57" s="15"/>
       <c r="R57" s="15"/>
       <c r="S57" s="16"/>
     </row>
-    <row r="58" spans="9:19">
+    <row r="58" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I58" s="15"/>
       <c r="R58" s="15"/>
       <c r="S58" s="16"/>
     </row>
-    <row r="59" spans="9:19">
+    <row r="59" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I59" s="15"/>
       <c r="R59" s="15"/>
       <c r="S59" s="16"/>
     </row>
-    <row r="60" spans="9:19">
+    <row r="60" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I60" s="15"/>
       <c r="R60" s="15"/>
       <c r="S60" s="16"/>
     </row>
-    <row r="61" spans="9:19">
+    <row r="61" spans="9:19" x14ac:dyDescent="0.2">
       <c r="I61" s="15"/>
       <c r="R61" s="15"/>
       <c r="S61" s="16"/>
     </row>
-    <row r="62" spans="9:19">
+    <row r="62" spans="9:19" x14ac:dyDescent="0.2">
       <c r="R62" s="15"/>
       <c r="S62" s="16"/>
     </row>
-    <row r="63" spans="9:19">
+    <row r="63" spans="9:19" x14ac:dyDescent="0.2">
       <c r="R63" s="15"/>
     </row>
-    <row r="64" spans="9:19">
+    <row r="64" spans="9:19" x14ac:dyDescent="0.2">
       <c r="R64" s="15"/>
     </row>
-    <row r="65" spans="18:18">
+    <row r="65" spans="18:18" x14ac:dyDescent="0.2">
       <c r="R65" s="15"/>
     </row>
   </sheetData>
@@ -5093,9 +5214,9 @@
       <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>16</v>
       </c>
@@ -5140,7 +5261,7 @@
       <c r="X1" s="24"/>
       <c r="Y1" s="25"/>
     </row>
-    <row r="2" spans="1:28" ht="16" thickBot="1">
+    <row r="2" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22"/>
       <c r="B2" s="8" t="s">
         <v>18</v>
@@ -5215,7 +5336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -5294,7 +5415,7 @@
       <c r="Z3" s="17"/>
       <c r="AB3" s="7"/>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -5373,7 +5494,7 @@
       <c r="Z4" s="17"/>
       <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -5452,7 +5573,7 @@
       <c r="Z5" s="17"/>
       <c r="AB5" s="7"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -5531,7 +5652,7 @@
       <c r="Z6" s="17"/>
       <c r="AB6" s="7"/>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -5610,7 +5731,7 @@
       <c r="Z7" s="17"/>
       <c r="AB7" s="7"/>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -5689,7 +5810,7 @@
       <c r="Z8" s="17"/>
       <c r="AB8" s="7"/>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -5768,7 +5889,7 @@
       <c r="Z9" s="17"/>
       <c r="AB9" s="7"/>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -5847,7 +5968,7 @@
       <c r="Z10" s="17"/>
       <c r="AB10" s="7"/>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -5926,7 +6047,7 @@
       <c r="Z11" s="17"/>
       <c r="AB11" s="7"/>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6005,7 +6126,7 @@
       <c r="Z12" s="17"/>
       <c r="AB12" s="7"/>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -6084,7 +6205,7 @@
       <c r="Z13" s="17"/>
       <c r="AB13" s="7"/>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -6163,7 +6284,7 @@
       <c r="Z14" s="17"/>
       <c r="AB14" s="7"/>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -6242,7 +6363,7 @@
       <c r="Z15" s="17"/>
       <c r="AB15" s="7"/>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -6321,7 +6442,7 @@
       <c r="Z16" s="17"/>
       <c r="AB16" s="7"/>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -6400,7 +6521,7 @@
       <c r="Z17" s="17"/>
       <c r="AB17" s="7"/>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -6473,7 +6594,7 @@
       <c r="Z18" s="17"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -6526,7 +6647,7 @@
       <c r="X19" s="4"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -6579,7 +6700,7 @@
       <c r="X20" s="4"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -6626,7 +6747,7 @@
       <c r="X21" s="4"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -6673,7 +6794,7 @@
       <c r="X22" s="4"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -6720,7 +6841,7 @@
       <c r="X23" s="4"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -6767,7 +6888,7 @@
       <c r="X24" s="4"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -6808,7 +6929,7 @@
       <c r="X25" s="4"/>
       <c r="Y25" s="5"/>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -6849,7 +6970,7 @@
       <c r="X26" s="4"/>
       <c r="Y26" s="5"/>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -6884,7 +7005,7 @@
       <c r="X27" s="4"/>
       <c r="Y27" s="5"/>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -6913,7 +7034,7 @@
       <c r="X28" s="4"/>
       <c r="Y28" s="5"/>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -6942,7 +7063,7 @@
       <c r="X29" s="4"/>
       <c r="Y29" s="5"/>
     </row>
-    <row r="30" spans="1:28" ht="16" thickBot="1">
+    <row r="30" spans="1:28" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>28</v>
       </c>
@@ -6971,148 +7092,148 @@
       <c r="X30" s="9"/>
       <c r="Y30" s="10"/>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="I32" s="15"/>
       <c r="S32" s="15"/>
       <c r="T32" s="16"/>
     </row>
-    <row r="33" spans="9:20">
+    <row r="33" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I33" s="15"/>
       <c r="S33" s="15"/>
       <c r="T33" s="16"/>
     </row>
-    <row r="34" spans="9:20">
+    <row r="34" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I34" s="15"/>
       <c r="S34" s="15"/>
       <c r="T34" s="16"/>
     </row>
-    <row r="35" spans="9:20">
+    <row r="35" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I35" s="15"/>
       <c r="S35" s="15"/>
       <c r="T35" s="16"/>
     </row>
-    <row r="36" spans="9:20">
+    <row r="36" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I36" s="15"/>
       <c r="S36" s="15"/>
       <c r="T36" s="16"/>
     </row>
-    <row r="37" spans="9:20">
+    <row r="37" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I37" s="15"/>
       <c r="S37" s="15"/>
       <c r="T37" s="16"/>
     </row>
-    <row r="38" spans="9:20">
+    <row r="38" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I38" s="15"/>
       <c r="S38" s="15"/>
       <c r="T38" s="16"/>
     </row>
-    <row r="39" spans="9:20">
+    <row r="39" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I39" s="15"/>
       <c r="S39" s="15"/>
       <c r="T39" s="16"/>
     </row>
-    <row r="40" spans="9:20">
+    <row r="40" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I40" s="15"/>
       <c r="S40" s="15"/>
       <c r="T40" s="16"/>
     </row>
-    <row r="41" spans="9:20">
+    <row r="41" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I41" s="15"/>
       <c r="S41" s="15"/>
       <c r="T41" s="16"/>
     </row>
-    <row r="42" spans="9:20">
+    <row r="42" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I42" s="15"/>
       <c r="S42" s="15"/>
       <c r="T42" s="16"/>
     </row>
-    <row r="43" spans="9:20">
+    <row r="43" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I43" s="15"/>
       <c r="S43" s="15"/>
       <c r="T43" s="16"/>
     </row>
-    <row r="44" spans="9:20">
+    <row r="44" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I44" s="15"/>
       <c r="S44" s="15"/>
       <c r="T44" s="16"/>
     </row>
-    <row r="45" spans="9:20">
+    <row r="45" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I45" s="15"/>
       <c r="S45" s="15"/>
       <c r="T45" s="16"/>
     </row>
-    <row r="46" spans="9:20">
+    <row r="46" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I46" s="15"/>
       <c r="S46" s="15"/>
       <c r="T46" s="16"/>
     </row>
-    <row r="47" spans="9:20">
+    <row r="47" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I47" s="15"/>
       <c r="S47" s="15"/>
       <c r="T47" s="16"/>
     </row>
-    <row r="48" spans="9:20">
+    <row r="48" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I48" s="15"/>
       <c r="S48" s="15"/>
       <c r="T48" s="16"/>
     </row>
-    <row r="49" spans="9:20">
+    <row r="49" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I49" s="15"/>
       <c r="S49" s="15"/>
       <c r="T49" s="16"/>
     </row>
-    <row r="50" spans="9:20">
+    <row r="50" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I50" s="15"/>
       <c r="S50" s="15"/>
       <c r="T50" s="16"/>
     </row>
-    <row r="51" spans="9:20">
+    <row r="51" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I51" s="15"/>
       <c r="S51" s="15"/>
       <c r="T51" s="16"/>
     </row>
-    <row r="52" spans="9:20">
+    <row r="52" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I52" s="15"/>
       <c r="S52" s="15"/>
       <c r="T52" s="16"/>
     </row>
-    <row r="53" spans="9:20">
+    <row r="53" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I53" s="15"/>
       <c r="S53" s="15"/>
       <c r="T53" s="16"/>
     </row>
-    <row r="54" spans="9:20">
+    <row r="54" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I54" s="15"/>
       <c r="S54" s="15"/>
       <c r="T54" s="16"/>
     </row>
-    <row r="55" spans="9:20">
+    <row r="55" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I55" s="15"/>
       <c r="S55" s="15"/>
       <c r="T55" s="16"/>
     </row>
-    <row r="56" spans="9:20">
+    <row r="56" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I56" s="15"/>
       <c r="S56" s="15"/>
       <c r="T56" s="16"/>
     </row>
-    <row r="57" spans="9:20">
+    <row r="57" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I57" s="15"/>
       <c r="S57" s="15"/>
     </row>
-    <row r="58" spans="9:20">
+    <row r="58" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I58" s="15"/>
       <c r="S58" s="15"/>
     </row>
-    <row r="59" spans="9:20">
+    <row r="59" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I59" s="15"/>
       <c r="S59" s="15"/>
     </row>
-    <row r="60" spans="9:20">
+    <row r="60" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I60" s="15"/>
       <c r="S60" s="15"/>
     </row>
-    <row r="61" spans="9:20">
+    <row r="61" spans="9:20" x14ac:dyDescent="0.2">
       <c r="I61" s="15"/>
     </row>
   </sheetData>
@@ -7129,4 +7250,3099 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABB26D70-89A7-EA4A-9E0A-F8C3AC05801A}">
+  <dimension ref="A1:AI96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="AB56" sqref="AB56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A1" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="P1" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="X1" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+    </row>
+    <row r="2" spans="1:35" ht="80" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="X2" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y2" s="33" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z2" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" s="32"/>
+    </row>
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A3" s="29">
+        <v>1</v>
+      </c>
+      <c r="B3" s="29">
+        <v>1</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="P3" s="27">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>1</v>
+      </c>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27">
+        <v>0</v>
+      </c>
+      <c r="U3" s="27">
+        <v>0</v>
+      </c>
+      <c r="V3" s="27">
+        <v>0</v>
+      </c>
+      <c r="X3" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27"/>
+      <c r="AE3" s="26"/>
+      <c r="AF3" s="26"/>
+      <c r="AG3" s="26"/>
+      <c r="AH3" s="26"/>
+      <c r="AI3" s="26"/>
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A4" s="29">
+        <v>2</v>
+      </c>
+      <c r="B4" s="29">
+        <v>1</v>
+      </c>
+      <c r="C4" s="29">
+        <v>1</v>
+      </c>
+      <c r="D4" s="29">
+        <v>1</v>
+      </c>
+      <c r="E4" s="29">
+        <v>1</v>
+      </c>
+      <c r="F4" s="29">
+        <v>1</v>
+      </c>
+      <c r="G4" s="29">
+        <v>1</v>
+      </c>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="P4" s="27">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="27">
+        <v>1</v>
+      </c>
+      <c r="R4" s="27">
+        <v>1</v>
+      </c>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27">
+        <v>1</v>
+      </c>
+      <c r="U4" s="27">
+        <v>0</v>
+      </c>
+      <c r="V4" s="27">
+        <v>1</v>
+      </c>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="27"/>
+      <c r="AE4" s="26"/>
+      <c r="AF4" s="26"/>
+      <c r="AG4" s="26"/>
+      <c r="AH4" s="26"/>
+      <c r="AI4" s="26"/>
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A5" s="29">
+        <v>3</v>
+      </c>
+      <c r="B5" s="29">
+        <v>1</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29">
+        <v>1</v>
+      </c>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="P5" s="27">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>1</v>
+      </c>
+      <c r="R5" s="27"/>
+      <c r="S5" s="27"/>
+      <c r="T5" s="27">
+        <v>0</v>
+      </c>
+      <c r="U5" s="27">
+        <v>0</v>
+      </c>
+      <c r="V5" s="27">
+        <v>1</v>
+      </c>
+      <c r="X5" s="27"/>
+      <c r="Y5" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="27"/>
+      <c r="AE5" s="26"/>
+      <c r="AF5" s="26"/>
+      <c r="AG5" s="26"/>
+      <c r="AH5" s="26"/>
+      <c r="AI5" s="26"/>
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A6" s="29">
+        <v>4</v>
+      </c>
+      <c r="B6" s="29">
+        <v>1</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29">
+        <v>1</v>
+      </c>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="P6" s="27">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="27">
+        <v>1</v>
+      </c>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27">
+        <v>0</v>
+      </c>
+      <c r="U6" s="27">
+        <v>0</v>
+      </c>
+      <c r="V6" s="27">
+        <v>1</v>
+      </c>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="26"/>
+      <c r="AI6" s="26"/>
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A7" s="29">
+        <v>5</v>
+      </c>
+      <c r="B7" s="29">
+        <v>1</v>
+      </c>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29">
+        <v>1</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29">
+        <v>1</v>
+      </c>
+      <c r="J7" s="29">
+        <v>1</v>
+      </c>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="P7" s="27">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="27">
+        <v>1</v>
+      </c>
+      <c r="R7" s="27">
+        <v>1</v>
+      </c>
+      <c r="S7" s="27">
+        <v>1</v>
+      </c>
+      <c r="T7" s="27">
+        <v>1</v>
+      </c>
+      <c r="U7" s="27">
+        <v>0</v>
+      </c>
+      <c r="V7" s="27">
+        <v>0</v>
+      </c>
+      <c r="X7" s="27"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="27"/>
+      <c r="AA7" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="26"/>
+      <c r="AF7" s="26"/>
+      <c r="AG7" s="26"/>
+      <c r="AH7" s="26"/>
+      <c r="AI7" s="26"/>
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A8" s="29">
+        <v>6</v>
+      </c>
+      <c r="B8" s="29">
+        <v>1</v>
+      </c>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29">
+        <v>1</v>
+      </c>
+      <c r="L8" s="29">
+        <v>1</v>
+      </c>
+      <c r="M8" s="29">
+        <v>1</v>
+      </c>
+      <c r="N8" s="29">
+        <v>1</v>
+      </c>
+      <c r="P8" s="27">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="27">
+        <v>1</v>
+      </c>
+      <c r="R8" s="27"/>
+      <c r="S8" s="27"/>
+      <c r="T8" s="27">
+        <v>0</v>
+      </c>
+      <c r="U8" s="27">
+        <v>1</v>
+      </c>
+      <c r="V8" s="27">
+        <v>0</v>
+      </c>
+      <c r="X8" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="27"/>
+      <c r="Z8" s="27"/>
+      <c r="AA8" s="27"/>
+      <c r="AE8" s="26"/>
+      <c r="AF8" s="26"/>
+      <c r="AG8" s="26"/>
+      <c r="AH8" s="26"/>
+      <c r="AI8" s="26"/>
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A9" s="29">
+        <v>7</v>
+      </c>
+      <c r="B9" s="29">
+        <v>1</v>
+      </c>
+      <c r="C9" s="29">
+        <v>1</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="P9" s="27">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="27">
+        <v>1</v>
+      </c>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="27">
+        <v>0</v>
+      </c>
+      <c r="U9" s="27">
+        <v>0</v>
+      </c>
+      <c r="V9" s="27">
+        <v>1</v>
+      </c>
+      <c r="X9" s="27"/>
+      <c r="Y9" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="27"/>
+      <c r="AA9" s="27"/>
+      <c r="AE9" s="26"/>
+      <c r="AF9" s="26"/>
+      <c r="AG9" s="26"/>
+      <c r="AH9" s="26"/>
+      <c r="AI9" s="26"/>
+    </row>
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A10" s="29">
+        <v>8</v>
+      </c>
+      <c r="B10" s="29">
+        <v>1</v>
+      </c>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29">
+        <v>1</v>
+      </c>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="P10" s="27">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="27">
+        <v>1</v>
+      </c>
+      <c r="R10" s="27"/>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27">
+        <v>0</v>
+      </c>
+      <c r="U10" s="27">
+        <v>0</v>
+      </c>
+      <c r="V10" s="27">
+        <v>1</v>
+      </c>
+      <c r="X10" s="27"/>
+      <c r="Y10" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="27"/>
+      <c r="AA10" s="27"/>
+      <c r="AE10" s="26"/>
+      <c r="AF10" s="26"/>
+      <c r="AG10" s="26"/>
+      <c r="AH10" s="26"/>
+      <c r="AI10" s="26"/>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A11" s="29">
+        <v>9</v>
+      </c>
+      <c r="B11" s="29">
+        <v>1</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="P11" s="27">
+        <v>9</v>
+      </c>
+      <c r="Q11" s="27">
+        <v>1</v>
+      </c>
+      <c r="R11" s="27"/>
+      <c r="S11" s="27"/>
+      <c r="T11" s="27">
+        <v>0</v>
+      </c>
+      <c r="U11" s="27">
+        <v>0</v>
+      </c>
+      <c r="V11" s="27">
+        <v>0</v>
+      </c>
+      <c r="X11" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="27"/>
+      <c r="Z11" s="27"/>
+      <c r="AA11" s="27"/>
+      <c r="AE11" s="26"/>
+      <c r="AF11" s="26"/>
+      <c r="AG11" s="26"/>
+      <c r="AH11" s="26"/>
+      <c r="AI11" s="26"/>
+    </row>
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A12" s="29">
+        <v>10</v>
+      </c>
+      <c r="B12" s="29">
+        <v>1</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="P12" s="27">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="27">
+        <v>1</v>
+      </c>
+      <c r="R12" s="27"/>
+      <c r="S12" s="27"/>
+      <c r="T12" s="27">
+        <v>0</v>
+      </c>
+      <c r="U12" s="27">
+        <v>0</v>
+      </c>
+      <c r="V12" s="27">
+        <v>0</v>
+      </c>
+      <c r="X12" s="27">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="27"/>
+      <c r="Z12" s="27"/>
+      <c r="AA12" s="27"/>
+      <c r="AE12" s="26"/>
+      <c r="AF12" s="26"/>
+      <c r="AG12" s="26"/>
+      <c r="AH12" s="26"/>
+      <c r="AI12" s="26"/>
+    </row>
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>11</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1</v>
+      </c>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29">
+        <v>1</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29">
+        <v>1</v>
+      </c>
+      <c r="J13" s="29">
+        <v>1</v>
+      </c>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="P13" s="27">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="27">
+        <v>1</v>
+      </c>
+      <c r="R13" s="27">
+        <v>1</v>
+      </c>
+      <c r="S13" s="27">
+        <v>1</v>
+      </c>
+      <c r="T13" s="27">
+        <v>1</v>
+      </c>
+      <c r="U13" s="27">
+        <v>0</v>
+      </c>
+      <c r="V13" s="27">
+        <v>0</v>
+      </c>
+      <c r="X13" s="27"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="27"/>
+      <c r="AA13" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26"/>
+    </row>
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A14" s="29">
+        <v>12</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1</v>
+      </c>
+      <c r="C14" s="29">
+        <v>1</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="P14" s="27">
+        <v>12</v>
+      </c>
+      <c r="Q14" s="27">
+        <v>1</v>
+      </c>
+      <c r="R14" s="27"/>
+      <c r="S14" s="27"/>
+      <c r="T14" s="27">
+        <v>0</v>
+      </c>
+      <c r="U14" s="27">
+        <v>0</v>
+      </c>
+      <c r="V14" s="27">
+        <v>1</v>
+      </c>
+      <c r="X14" s="27"/>
+      <c r="Y14" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="27"/>
+      <c r="AA14" s="27"/>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>13</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="P15" s="27">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="27">
+        <v>1</v>
+      </c>
+      <c r="R15" s="27"/>
+      <c r="S15" s="27"/>
+      <c r="T15" s="27">
+        <v>0</v>
+      </c>
+      <c r="U15" s="27">
+        <v>0</v>
+      </c>
+      <c r="V15" s="27">
+        <v>1</v>
+      </c>
+      <c r="X15" s="27"/>
+      <c r="Y15" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="27"/>
+      <c r="AA15" s="27"/>
+      <c r="AE15" s="26"/>
+      <c r="AF15" s="26"/>
+      <c r="AG15" s="26"/>
+      <c r="AH15" s="26"/>
+      <c r="AI15" s="26"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A16" s="29">
+        <v>14</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1</v>
+      </c>
+      <c r="C16" s="29">
+        <v>1</v>
+      </c>
+      <c r="D16" s="29">
+        <v>1</v>
+      </c>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
+      <c r="F16" s="29">
+        <v>1</v>
+      </c>
+      <c r="G16" s="29">
+        <v>1</v>
+      </c>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="P16" s="27">
+        <v>14</v>
+      </c>
+      <c r="Q16" s="27">
+        <v>1</v>
+      </c>
+      <c r="R16" s="27">
+        <v>1</v>
+      </c>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27">
+        <v>1</v>
+      </c>
+      <c r="U16" s="27">
+        <v>0</v>
+      </c>
+      <c r="V16" s="27">
+        <v>1</v>
+      </c>
+      <c r="X16" s="27"/>
+      <c r="Y16" s="27"/>
+      <c r="Z16" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="27"/>
+      <c r="AE16" s="26"/>
+      <c r="AF16" s="26"/>
+      <c r="AG16" s="26"/>
+      <c r="AH16" s="26"/>
+      <c r="AI16" s="26"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A17" s="29">
+        <v>15</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29">
+        <v>1</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29">
+        <v>1</v>
+      </c>
+      <c r="J17" s="29">
+        <v>1</v>
+      </c>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="P17" s="27">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="27">
+        <v>1</v>
+      </c>
+      <c r="R17" s="27">
+        <v>1</v>
+      </c>
+      <c r="S17" s="27">
+        <v>1</v>
+      </c>
+      <c r="T17" s="27">
+        <v>1</v>
+      </c>
+      <c r="U17" s="27">
+        <v>0</v>
+      </c>
+      <c r="V17" s="27">
+        <v>0</v>
+      </c>
+      <c r="X17" s="27"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="27"/>
+      <c r="AA17" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="26"/>
+      <c r="AF17" s="26"/>
+      <c r="AG17" s="26"/>
+      <c r="AH17" s="26"/>
+      <c r="AI17" s="26"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A18" s="29">
+        <v>16</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1</v>
+      </c>
+      <c r="C18" s="29">
+        <v>1</v>
+      </c>
+      <c r="D18" s="29">
+        <v>1</v>
+      </c>
+      <c r="E18" s="29">
+        <v>1</v>
+      </c>
+      <c r="F18" s="29">
+        <v>1</v>
+      </c>
+      <c r="G18" s="29">
+        <v>1</v>
+      </c>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="P18" s="27">
+        <v>16</v>
+      </c>
+      <c r="Q18" s="27">
+        <v>1</v>
+      </c>
+      <c r="R18" s="27">
+        <v>1</v>
+      </c>
+      <c r="S18" s="27"/>
+      <c r="T18" s="27">
+        <v>1</v>
+      </c>
+      <c r="U18" s="27">
+        <v>0</v>
+      </c>
+      <c r="V18" s="27">
+        <v>1</v>
+      </c>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="27"/>
+      <c r="AE18" s="26"/>
+      <c r="AF18" s="26"/>
+      <c r="AG18" s="26"/>
+      <c r="AH18" s="26"/>
+      <c r="AI18" s="26"/>
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A19" s="29">
+        <v>17</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1</v>
+      </c>
+      <c r="C19" s="29">
+        <v>1</v>
+      </c>
+      <c r="D19" s="29">
+        <v>1</v>
+      </c>
+      <c r="E19" s="29">
+        <v>1</v>
+      </c>
+      <c r="F19" s="29">
+        <v>1</v>
+      </c>
+      <c r="G19" s="29">
+        <v>1</v>
+      </c>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="P19" s="27">
+        <v>17</v>
+      </c>
+      <c r="Q19" s="27">
+        <v>1</v>
+      </c>
+      <c r="R19" s="27">
+        <v>1</v>
+      </c>
+      <c r="S19" s="27"/>
+      <c r="T19" s="27">
+        <v>1</v>
+      </c>
+      <c r="U19" s="27">
+        <v>0</v>
+      </c>
+      <c r="V19" s="27">
+        <v>1</v>
+      </c>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="27"/>
+      <c r="AE19" s="26"/>
+      <c r="AF19" s="26"/>
+      <c r="AG19" s="26"/>
+      <c r="AH19" s="26"/>
+      <c r="AI19" s="26"/>
+    </row>
+    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A20" s="29">
+        <v>18</v>
+      </c>
+      <c r="B20" s="29">
+        <v>1</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29">
+        <v>1</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29">
+        <v>1</v>
+      </c>
+      <c r="J20" s="29">
+        <v>1</v>
+      </c>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="P20" s="27">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="27">
+        <v>1</v>
+      </c>
+      <c r="R20" s="27">
+        <v>1</v>
+      </c>
+      <c r="S20" s="27">
+        <v>1</v>
+      </c>
+      <c r="T20" s="27">
+        <v>1</v>
+      </c>
+      <c r="U20" s="27">
+        <v>0</v>
+      </c>
+      <c r="V20" s="27">
+        <v>0</v>
+      </c>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="27"/>
+      <c r="AA20" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="26"/>
+      <c r="AF20" s="26"/>
+      <c r="AG20" s="26"/>
+      <c r="AH20" s="26"/>
+      <c r="AI20" s="26"/>
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A21" s="29">
+        <v>19</v>
+      </c>
+      <c r="B21" s="29">
+        <v>1</v>
+      </c>
+      <c r="C21" s="29">
+        <v>1</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="P21" s="27">
+        <v>19</v>
+      </c>
+      <c r="Q21" s="27">
+        <v>1</v>
+      </c>
+      <c r="R21" s="27"/>
+      <c r="S21" s="27"/>
+      <c r="T21" s="27">
+        <v>0</v>
+      </c>
+      <c r="U21" s="27">
+        <v>0</v>
+      </c>
+      <c r="V21" s="27">
+        <v>1</v>
+      </c>
+      <c r="X21" s="27"/>
+      <c r="Y21" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="27"/>
+      <c r="AA21" s="27"/>
+      <c r="AE21" s="26"/>
+      <c r="AF21" s="26"/>
+      <c r="AG21" s="26"/>
+      <c r="AH21" s="26"/>
+      <c r="AI21" s="26"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A22" s="29">
+        <v>20</v>
+      </c>
+      <c r="B22" s="29">
+        <v>1</v>
+      </c>
+      <c r="C22" s="29">
+        <v>1</v>
+      </c>
+      <c r="D22" s="29">
+        <v>1</v>
+      </c>
+      <c r="E22" s="29">
+        <v>1</v>
+      </c>
+      <c r="F22" s="29">
+        <v>1</v>
+      </c>
+      <c r="G22" s="29">
+        <v>1</v>
+      </c>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="P22" s="27">
+        <v>20</v>
+      </c>
+      <c r="Q22" s="27">
+        <v>1</v>
+      </c>
+      <c r="R22" s="27">
+        <v>1</v>
+      </c>
+      <c r="S22" s="27"/>
+      <c r="T22" s="27">
+        <v>1</v>
+      </c>
+      <c r="U22" s="27">
+        <v>0</v>
+      </c>
+      <c r="V22" s="27">
+        <v>1</v>
+      </c>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="27"/>
+      <c r="AE22" s="26"/>
+      <c r="AF22" s="26"/>
+      <c r="AG22" s="26"/>
+      <c r="AH22" s="26"/>
+      <c r="AI22" s="26"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A23" s="29">
+        <v>21</v>
+      </c>
+      <c r="B23" s="29">
+        <v>1</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29">
+        <v>1</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29">
+        <v>1</v>
+      </c>
+      <c r="J23" s="29">
+        <v>1</v>
+      </c>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="P23" s="27">
+        <v>21</v>
+      </c>
+      <c r="Q23" s="27">
+        <v>1</v>
+      </c>
+      <c r="R23" s="27">
+        <v>1</v>
+      </c>
+      <c r="S23" s="27">
+        <v>1</v>
+      </c>
+      <c r="T23" s="27">
+        <v>1</v>
+      </c>
+      <c r="U23" s="27">
+        <v>0</v>
+      </c>
+      <c r="V23" s="27">
+        <v>0</v>
+      </c>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE23" s="26"/>
+      <c r="AF23" s="26"/>
+      <c r="AG23" s="26"/>
+      <c r="AH23" s="26"/>
+      <c r="AI23" s="26"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A24" s="29">
+        <v>22</v>
+      </c>
+      <c r="B24" s="29">
+        <v>1</v>
+      </c>
+      <c r="C24" s="29">
+        <v>1</v>
+      </c>
+      <c r="D24" s="29">
+        <v>1</v>
+      </c>
+      <c r="E24" s="29">
+        <v>1</v>
+      </c>
+      <c r="F24" s="29">
+        <v>1</v>
+      </c>
+      <c r="G24" s="29">
+        <v>1</v>
+      </c>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="P24" s="27">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="27">
+        <v>1</v>
+      </c>
+      <c r="R24" s="27">
+        <v>1</v>
+      </c>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27">
+        <v>1</v>
+      </c>
+      <c r="U24" s="27">
+        <v>0</v>
+      </c>
+      <c r="V24" s="27">
+        <v>1</v>
+      </c>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="27"/>
+      <c r="AE24" s="26"/>
+      <c r="AF24" s="26"/>
+      <c r="AG24" s="26"/>
+      <c r="AH24" s="26"/>
+      <c r="AI24" s="26"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A25" s="29">
+        <v>23</v>
+      </c>
+      <c r="B25" s="29">
+        <v>1</v>
+      </c>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29">
+        <v>1</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29">
+        <v>1</v>
+      </c>
+      <c r="J25" s="29">
+        <v>1</v>
+      </c>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="P25" s="27">
+        <v>23</v>
+      </c>
+      <c r="Q25" s="27">
+        <v>1</v>
+      </c>
+      <c r="R25" s="27">
+        <v>1</v>
+      </c>
+      <c r="S25" s="27">
+        <v>1</v>
+      </c>
+      <c r="T25" s="27">
+        <v>1</v>
+      </c>
+      <c r="U25" s="27">
+        <v>0</v>
+      </c>
+      <c r="V25" s="27">
+        <v>0</v>
+      </c>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
+      <c r="AA25" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE25" s="26"/>
+      <c r="AF25" s="26"/>
+      <c r="AG25" s="26"/>
+      <c r="AH25" s="26"/>
+      <c r="AI25" s="26"/>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A26" s="29">
+        <v>24</v>
+      </c>
+      <c r="B26" s="29">
+        <v>1</v>
+      </c>
+      <c r="C26" s="29">
+        <v>1</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="P26" s="27">
+        <v>24</v>
+      </c>
+      <c r="Q26" s="27">
+        <v>1</v>
+      </c>
+      <c r="R26" s="27"/>
+      <c r="S26" s="27"/>
+      <c r="T26" s="27">
+        <v>0</v>
+      </c>
+      <c r="U26" s="27">
+        <v>0</v>
+      </c>
+      <c r="V26" s="27">
+        <v>1</v>
+      </c>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="27"/>
+      <c r="AA26" s="27"/>
+      <c r="AE26" s="26"/>
+      <c r="AF26" s="26"/>
+      <c r="AG26" s="26"/>
+      <c r="AH26" s="26"/>
+      <c r="AI26" s="26"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A27" s="29">
+        <v>25</v>
+      </c>
+      <c r="B27" s="29">
+        <v>1</v>
+      </c>
+      <c r="C27" s="29">
+        <v>1</v>
+      </c>
+      <c r="D27" s="29">
+        <v>1</v>
+      </c>
+      <c r="E27" s="29">
+        <v>1</v>
+      </c>
+      <c r="F27" s="29">
+        <v>1</v>
+      </c>
+      <c r="G27" s="29">
+        <v>1</v>
+      </c>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="P27" s="27">
+        <v>25</v>
+      </c>
+      <c r="Q27" s="27">
+        <v>1</v>
+      </c>
+      <c r="R27" s="27">
+        <v>1</v>
+      </c>
+      <c r="S27" s="27"/>
+      <c r="T27" s="27">
+        <v>1</v>
+      </c>
+      <c r="U27" s="27">
+        <v>0</v>
+      </c>
+      <c r="V27" s="27">
+        <v>1</v>
+      </c>
+      <c r="X27" s="27"/>
+      <c r="Y27" s="27"/>
+      <c r="Z27" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="27"/>
+      <c r="AE27" s="26"/>
+      <c r="AF27" s="26"/>
+      <c r="AG27" s="26"/>
+      <c r="AH27" s="26"/>
+      <c r="AI27" s="26"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A28" s="29">
+        <v>26</v>
+      </c>
+      <c r="B28" s="29">
+        <v>1</v>
+      </c>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29">
+        <v>1</v>
+      </c>
+      <c r="L28" s="29">
+        <v>1</v>
+      </c>
+      <c r="M28" s="29">
+        <v>1</v>
+      </c>
+      <c r="N28" s="29">
+        <v>1</v>
+      </c>
+      <c r="P28" s="27">
+        <v>26</v>
+      </c>
+      <c r="Q28" s="27">
+        <v>1</v>
+      </c>
+      <c r="R28" s="27"/>
+      <c r="S28" s="27"/>
+      <c r="T28" s="27">
+        <v>0</v>
+      </c>
+      <c r="U28" s="27">
+        <v>1</v>
+      </c>
+      <c r="V28" s="27">
+        <v>0</v>
+      </c>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
+      <c r="AA28" s="27"/>
+      <c r="AE28" s="26"/>
+      <c r="AF28" s="26"/>
+      <c r="AG28" s="26"/>
+      <c r="AH28" s="26"/>
+      <c r="AI28" s="26"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A29" s="29">
+        <v>27</v>
+      </c>
+      <c r="B29" s="29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="29">
+        <v>1</v>
+      </c>
+      <c r="D29" s="29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="29">
+        <v>1</v>
+      </c>
+      <c r="G29" s="29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="P29" s="27">
+        <v>27</v>
+      </c>
+      <c r="Q29" s="27">
+        <v>1</v>
+      </c>
+      <c r="R29" s="27">
+        <v>1</v>
+      </c>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27">
+        <v>1</v>
+      </c>
+      <c r="U29" s="27">
+        <v>0</v>
+      </c>
+      <c r="V29" s="27">
+        <v>1</v>
+      </c>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="27"/>
+      <c r="Z29" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="27"/>
+      <c r="AE29" s="26"/>
+      <c r="AF29" s="26"/>
+      <c r="AG29" s="26"/>
+      <c r="AH29" s="26"/>
+      <c r="AI29" s="26"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A30" s="29">
+        <v>28</v>
+      </c>
+      <c r="B30" s="29">
+        <v>1</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29">
+        <v>1</v>
+      </c>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29">
+        <v>1</v>
+      </c>
+      <c r="J30" s="29">
+        <v>1</v>
+      </c>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="P30" s="27">
+        <v>28</v>
+      </c>
+      <c r="Q30" s="27">
+        <v>1</v>
+      </c>
+      <c r="R30" s="27">
+        <v>1</v>
+      </c>
+      <c r="S30" s="27">
+        <v>1</v>
+      </c>
+      <c r="T30" s="27">
+        <v>1</v>
+      </c>
+      <c r="U30" s="27">
+        <v>0</v>
+      </c>
+      <c r="V30" s="27">
+        <v>0</v>
+      </c>
+      <c r="X30" s="27"/>
+      <c r="Y30" s="27"/>
+      <c r="Z30" s="27"/>
+      <c r="AA30" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE30" s="26"/>
+      <c r="AF30" s="26"/>
+      <c r="AG30" s="26"/>
+      <c r="AH30" s="26"/>
+      <c r="AI30" s="26"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A31" s="29">
+        <v>29</v>
+      </c>
+      <c r="B31" s="29">
+        <v>1</v>
+      </c>
+      <c r="C31" s="29">
+        <v>1</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="P31" s="27">
+        <v>29</v>
+      </c>
+      <c r="Q31" s="27">
+        <v>1</v>
+      </c>
+      <c r="R31" s="27"/>
+      <c r="S31" s="27"/>
+      <c r="T31" s="27">
+        <v>0</v>
+      </c>
+      <c r="U31" s="27">
+        <v>0</v>
+      </c>
+      <c r="V31" s="27">
+        <v>1</v>
+      </c>
+      <c r="X31" s="27"/>
+      <c r="Y31" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z31" s="27"/>
+      <c r="AA31" s="27"/>
+      <c r="AE31" s="26"/>
+      <c r="AF31" s="26"/>
+      <c r="AG31" s="26"/>
+      <c r="AH31" s="26"/>
+      <c r="AI31" s="26"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A32" s="29">
+        <v>30</v>
+      </c>
+      <c r="B32" s="29">
+        <v>1</v>
+      </c>
+      <c r="C32" s="29">
+        <v>1</v>
+      </c>
+      <c r="D32" s="29">
+        <v>1</v>
+      </c>
+      <c r="E32" s="29">
+        <v>1</v>
+      </c>
+      <c r="F32" s="29">
+        <v>1</v>
+      </c>
+      <c r="G32" s="29">
+        <v>1</v>
+      </c>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="P32" s="27">
+        <v>30</v>
+      </c>
+      <c r="Q32" s="27">
+        <v>1</v>
+      </c>
+      <c r="R32" s="27">
+        <v>1</v>
+      </c>
+      <c r="S32" s="27"/>
+      <c r="T32" s="27">
+        <v>1</v>
+      </c>
+      <c r="U32" s="27">
+        <v>0</v>
+      </c>
+      <c r="V32" s="27">
+        <v>1</v>
+      </c>
+      <c r="X32" s="27"/>
+      <c r="Y32" s="27"/>
+      <c r="Z32" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA32" s="27"/>
+      <c r="AE32" s="26"/>
+      <c r="AF32" s="26"/>
+      <c r="AG32" s="26"/>
+      <c r="AH32" s="26"/>
+      <c r="AI32" s="26"/>
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A33" s="29">
+        <v>31</v>
+      </c>
+      <c r="B33" s="29">
+        <v>1</v>
+      </c>
+      <c r="C33" s="29">
+        <v>1</v>
+      </c>
+      <c r="D33" s="29">
+        <v>1</v>
+      </c>
+      <c r="E33" s="29">
+        <v>1</v>
+      </c>
+      <c r="F33" s="29">
+        <v>1</v>
+      </c>
+      <c r="G33" s="29">
+        <v>1</v>
+      </c>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="P33" s="27">
+        <v>31</v>
+      </c>
+      <c r="Q33" s="27">
+        <v>1</v>
+      </c>
+      <c r="R33" s="27">
+        <v>1</v>
+      </c>
+      <c r="S33" s="27"/>
+      <c r="T33" s="27">
+        <v>1</v>
+      </c>
+      <c r="U33" s="27">
+        <v>0</v>
+      </c>
+      <c r="V33" s="27">
+        <v>1</v>
+      </c>
+      <c r="X33" s="27"/>
+      <c r="Y33" s="27"/>
+      <c r="Z33" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA33" s="27"/>
+      <c r="AE33" s="26"/>
+      <c r="AF33" s="26"/>
+      <c r="AG33" s="26"/>
+      <c r="AH33" s="26"/>
+      <c r="AI33" s="26"/>
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A34" s="29">
+        <v>32</v>
+      </c>
+      <c r="B34" s="29">
+        <v>1</v>
+      </c>
+      <c r="C34" s="29">
+        <v>1</v>
+      </c>
+      <c r="D34" s="29">
+        <v>1</v>
+      </c>
+      <c r="E34" s="29">
+        <v>1</v>
+      </c>
+      <c r="F34" s="29">
+        <v>1</v>
+      </c>
+      <c r="G34" s="29">
+        <v>1</v>
+      </c>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="P34" s="27">
+        <v>32</v>
+      </c>
+      <c r="Q34" s="27">
+        <v>1</v>
+      </c>
+      <c r="R34" s="27">
+        <v>1</v>
+      </c>
+      <c r="S34" s="27"/>
+      <c r="T34" s="27">
+        <v>1</v>
+      </c>
+      <c r="U34" s="27">
+        <v>0</v>
+      </c>
+      <c r="V34" s="27">
+        <v>1</v>
+      </c>
+      <c r="X34" s="27"/>
+      <c r="Y34" s="27"/>
+      <c r="Z34" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="27"/>
+      <c r="AE34" s="26"/>
+      <c r="AF34" s="26"/>
+      <c r="AG34" s="26"/>
+      <c r="AH34" s="26"/>
+      <c r="AI34" s="26"/>
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A35" s="29">
+        <v>33</v>
+      </c>
+      <c r="B35" s="29">
+        <v>1</v>
+      </c>
+      <c r="C35" s="29">
+        <v>1</v>
+      </c>
+      <c r="D35" s="29">
+        <v>1</v>
+      </c>
+      <c r="E35" s="29">
+        <v>1</v>
+      </c>
+      <c r="F35" s="29">
+        <v>1</v>
+      </c>
+      <c r="G35" s="29">
+        <v>1</v>
+      </c>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="P35" s="27">
+        <v>33</v>
+      </c>
+      <c r="Q35" s="27">
+        <v>1</v>
+      </c>
+      <c r="R35" s="27">
+        <v>1</v>
+      </c>
+      <c r="S35" s="27"/>
+      <c r="T35" s="27">
+        <v>1</v>
+      </c>
+      <c r="U35" s="27">
+        <v>0</v>
+      </c>
+      <c r="V35" s="27">
+        <v>1</v>
+      </c>
+      <c r="X35" s="27"/>
+      <c r="Y35" s="27"/>
+      <c r="Z35" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA35" s="27"/>
+      <c r="AE35" s="26"/>
+      <c r="AF35" s="26"/>
+      <c r="AG35" s="26"/>
+      <c r="AH35" s="26"/>
+      <c r="AI35" s="26"/>
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A36" s="29">
+        <v>34</v>
+      </c>
+      <c r="B36" s="29">
+        <v>1</v>
+      </c>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29">
+        <v>1</v>
+      </c>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29">
+        <v>1</v>
+      </c>
+      <c r="J36" s="29">
+        <v>1</v>
+      </c>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="P36" s="27">
+        <v>34</v>
+      </c>
+      <c r="Q36" s="27">
+        <v>1</v>
+      </c>
+      <c r="R36" s="27">
+        <v>1</v>
+      </c>
+      <c r="S36" s="27">
+        <v>1</v>
+      </c>
+      <c r="T36" s="27">
+        <v>1</v>
+      </c>
+      <c r="U36" s="27">
+        <v>0</v>
+      </c>
+      <c r="V36" s="27">
+        <v>0</v>
+      </c>
+      <c r="X36" s="27"/>
+      <c r="Y36" s="27"/>
+      <c r="Z36" s="27"/>
+      <c r="AA36" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE36" s="26"/>
+      <c r="AF36" s="26"/>
+      <c r="AG36" s="26"/>
+      <c r="AH36" s="26"/>
+      <c r="AI36" s="26"/>
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A37" s="29">
+        <v>35</v>
+      </c>
+      <c r="B37" s="29">
+        <v>1</v>
+      </c>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29">
+        <v>1</v>
+      </c>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29">
+        <v>1</v>
+      </c>
+      <c r="J37" s="29">
+        <v>1</v>
+      </c>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="P37" s="27">
+        <v>35</v>
+      </c>
+      <c r="Q37" s="27">
+        <v>1</v>
+      </c>
+      <c r="R37" s="27">
+        <v>1</v>
+      </c>
+      <c r="S37" s="27">
+        <v>1</v>
+      </c>
+      <c r="T37" s="27">
+        <v>1</v>
+      </c>
+      <c r="U37" s="27">
+        <v>0</v>
+      </c>
+      <c r="V37" s="27">
+        <v>0</v>
+      </c>
+      <c r="X37" s="27"/>
+      <c r="Y37" s="27"/>
+      <c r="Z37" s="27"/>
+      <c r="AA37" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE37" s="26"/>
+      <c r="AF37" s="26"/>
+      <c r="AG37" s="26"/>
+      <c r="AH37" s="26"/>
+      <c r="AI37" s="26"/>
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A38" s="29">
+        <v>36</v>
+      </c>
+      <c r="B38" s="29">
+        <v>1</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29">
+        <v>1</v>
+      </c>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29">
+        <v>1</v>
+      </c>
+      <c r="J38" s="29">
+        <v>1</v>
+      </c>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="P38" s="27">
+        <v>36</v>
+      </c>
+      <c r="Q38" s="27">
+        <v>1</v>
+      </c>
+      <c r="R38" s="27">
+        <v>1</v>
+      </c>
+      <c r="S38" s="27">
+        <v>1</v>
+      </c>
+      <c r="T38" s="27">
+        <v>1</v>
+      </c>
+      <c r="U38" s="27">
+        <v>0</v>
+      </c>
+      <c r="V38" s="27">
+        <v>0</v>
+      </c>
+      <c r="X38" s="27"/>
+      <c r="Y38" s="27"/>
+      <c r="Z38" s="27"/>
+      <c r="AA38" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE38" s="26"/>
+      <c r="AF38" s="26"/>
+      <c r="AG38" s="26"/>
+      <c r="AH38" s="26"/>
+      <c r="AI38" s="26"/>
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A39" s="29">
+        <v>37</v>
+      </c>
+      <c r="B39" s="29">
+        <v>1</v>
+      </c>
+      <c r="C39" s="29">
+        <v>1</v>
+      </c>
+      <c r="D39" s="29">
+        <v>1</v>
+      </c>
+      <c r="E39" s="29">
+        <v>1</v>
+      </c>
+      <c r="F39" s="29">
+        <v>1</v>
+      </c>
+      <c r="G39" s="29">
+        <v>1</v>
+      </c>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="P39" s="27">
+        <v>37</v>
+      </c>
+      <c r="Q39" s="27">
+        <v>1</v>
+      </c>
+      <c r="R39" s="27">
+        <v>1</v>
+      </c>
+      <c r="S39" s="27"/>
+      <c r="T39" s="27">
+        <v>1</v>
+      </c>
+      <c r="U39" s="27">
+        <v>0</v>
+      </c>
+      <c r="V39" s="27">
+        <v>1</v>
+      </c>
+      <c r="X39" s="27"/>
+      <c r="Y39" s="27"/>
+      <c r="Z39" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA39" s="27"/>
+      <c r="AE39" s="26"/>
+      <c r="AF39" s="26"/>
+      <c r="AG39" s="26"/>
+      <c r="AH39" s="26"/>
+      <c r="AI39" s="26"/>
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A40" s="29">
+        <v>38</v>
+      </c>
+      <c r="B40" s="29">
+        <v>1</v>
+      </c>
+      <c r="C40" s="29">
+        <v>1</v>
+      </c>
+      <c r="D40" s="29">
+        <v>1</v>
+      </c>
+      <c r="E40" s="29">
+        <v>1</v>
+      </c>
+      <c r="F40" s="29">
+        <v>1</v>
+      </c>
+      <c r="G40" s="29">
+        <v>1</v>
+      </c>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="P40" s="27">
+        <v>38</v>
+      </c>
+      <c r="Q40" s="27">
+        <v>1</v>
+      </c>
+      <c r="R40" s="27">
+        <v>1</v>
+      </c>
+      <c r="S40" s="27"/>
+      <c r="T40" s="27">
+        <v>1</v>
+      </c>
+      <c r="U40" s="27">
+        <v>0</v>
+      </c>
+      <c r="V40" s="27">
+        <v>1</v>
+      </c>
+      <c r="X40" s="27"/>
+      <c r="Y40" s="27"/>
+      <c r="Z40" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="27"/>
+      <c r="AE40" s="26"/>
+      <c r="AF40" s="26"/>
+      <c r="AG40" s="26"/>
+      <c r="AH40" s="26"/>
+      <c r="AI40" s="26"/>
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A41" s="29">
+        <v>39</v>
+      </c>
+      <c r="B41" s="29">
+        <v>1</v>
+      </c>
+      <c r="C41" s="29">
+        <v>1</v>
+      </c>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="P41" s="27">
+        <v>39</v>
+      </c>
+      <c r="Q41" s="27">
+        <v>1</v>
+      </c>
+      <c r="R41" s="27"/>
+      <c r="S41" s="27"/>
+      <c r="T41" s="27">
+        <v>0</v>
+      </c>
+      <c r="U41" s="27">
+        <v>0</v>
+      </c>
+      <c r="V41" s="27">
+        <v>1</v>
+      </c>
+      <c r="X41" s="27"/>
+      <c r="Y41" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z41" s="27"/>
+      <c r="AA41" s="27"/>
+      <c r="AE41" s="26"/>
+      <c r="AF41" s="26"/>
+      <c r="AG41" s="26"/>
+      <c r="AH41" s="26"/>
+      <c r="AI41" s="26"/>
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A42" s="29">
+        <v>40</v>
+      </c>
+      <c r="B42" s="29">
+        <v>1</v>
+      </c>
+      <c r="C42" s="29">
+        <v>1</v>
+      </c>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="P42" s="27">
+        <v>40</v>
+      </c>
+      <c r="Q42" s="27">
+        <v>1</v>
+      </c>
+      <c r="R42" s="27"/>
+      <c r="S42" s="27"/>
+      <c r="T42" s="27">
+        <v>0</v>
+      </c>
+      <c r="U42" s="27">
+        <v>0</v>
+      </c>
+      <c r="V42" s="27">
+        <v>1</v>
+      </c>
+      <c r="X42" s="27"/>
+      <c r="Y42" s="27">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="27"/>
+      <c r="AA42" s="27"/>
+      <c r="AE42" s="26"/>
+      <c r="AF42" s="26"/>
+      <c r="AG42" s="26"/>
+      <c r="AH42" s="26"/>
+      <c r="AI42" s="26"/>
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A43" s="29">
+        <v>41</v>
+      </c>
+      <c r="B43" s="29">
+        <v>1</v>
+      </c>
+      <c r="C43" s="29">
+        <v>1</v>
+      </c>
+      <c r="D43" s="29">
+        <v>1</v>
+      </c>
+      <c r="E43" s="29">
+        <v>1</v>
+      </c>
+      <c r="F43" s="29">
+        <v>1</v>
+      </c>
+      <c r="G43" s="29">
+        <v>1</v>
+      </c>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="P43" s="27">
+        <v>41</v>
+      </c>
+      <c r="Q43" s="27">
+        <v>1</v>
+      </c>
+      <c r="R43" s="27">
+        <v>1</v>
+      </c>
+      <c r="S43" s="27"/>
+      <c r="T43" s="27">
+        <v>1</v>
+      </c>
+      <c r="U43" s="27">
+        <v>0</v>
+      </c>
+      <c r="V43" s="27">
+        <v>1</v>
+      </c>
+      <c r="X43" s="27"/>
+      <c r="Y43" s="27"/>
+      <c r="Z43" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA43" s="27"/>
+      <c r="AE43" s="26"/>
+      <c r="AF43" s="26"/>
+      <c r="AG43" s="26"/>
+      <c r="AH43" s="26"/>
+      <c r="AI43" s="26"/>
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A44" s="29">
+        <v>42</v>
+      </c>
+      <c r="B44" s="29">
+        <v>1</v>
+      </c>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29">
+        <v>1</v>
+      </c>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29">
+        <v>1</v>
+      </c>
+      <c r="J44" s="29">
+        <v>1</v>
+      </c>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="P44" s="27">
+        <v>42</v>
+      </c>
+      <c r="Q44" s="27">
+        <v>1</v>
+      </c>
+      <c r="R44" s="27">
+        <v>1</v>
+      </c>
+      <c r="S44" s="27">
+        <v>1</v>
+      </c>
+      <c r="T44" s="27">
+        <v>1</v>
+      </c>
+      <c r="U44" s="27">
+        <v>0</v>
+      </c>
+      <c r="V44" s="27">
+        <v>0</v>
+      </c>
+      <c r="X44" s="27"/>
+      <c r="Y44" s="27"/>
+      <c r="Z44" s="27"/>
+      <c r="AA44" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE44" s="26"/>
+      <c r="AF44" s="26"/>
+      <c r="AG44" s="26"/>
+      <c r="AH44" s="26"/>
+      <c r="AI44" s="26"/>
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A45" s="29">
+        <v>43</v>
+      </c>
+      <c r="B45" s="29">
+        <v>1</v>
+      </c>
+      <c r="C45" s="29">
+        <v>1</v>
+      </c>
+      <c r="D45" s="29">
+        <v>1</v>
+      </c>
+      <c r="E45" s="29">
+        <v>1</v>
+      </c>
+      <c r="F45" s="29">
+        <v>1</v>
+      </c>
+      <c r="G45" s="29">
+        <v>1</v>
+      </c>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
+      <c r="P45" s="27">
+        <v>43</v>
+      </c>
+      <c r="Q45" s="27">
+        <v>1</v>
+      </c>
+      <c r="R45" s="27">
+        <v>1</v>
+      </c>
+      <c r="S45" s="27"/>
+      <c r="T45" s="27">
+        <v>1</v>
+      </c>
+      <c r="U45" s="27">
+        <v>0</v>
+      </c>
+      <c r="V45" s="27">
+        <v>1</v>
+      </c>
+      <c r="X45" s="27"/>
+      <c r="Y45" s="27"/>
+      <c r="Z45" s="27">
+        <v>1</v>
+      </c>
+      <c r="AA45" s="27"/>
+      <c r="AE45" s="26"/>
+      <c r="AF45" s="26"/>
+      <c r="AG45" s="26"/>
+      <c r="AH45" s="26"/>
+      <c r="AI45" s="26"/>
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A46" s="29">
+        <v>44</v>
+      </c>
+      <c r="B46" s="29">
+        <v>1</v>
+      </c>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29">
+        <v>1</v>
+      </c>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29">
+        <v>1</v>
+      </c>
+      <c r="J46" s="29">
+        <v>1</v>
+      </c>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="29"/>
+      <c r="N46" s="29"/>
+      <c r="P46" s="27">
+        <v>44</v>
+      </c>
+      <c r="Q46" s="27">
+        <v>1</v>
+      </c>
+      <c r="R46" s="27">
+        <v>1</v>
+      </c>
+      <c r="S46" s="27">
+        <v>1</v>
+      </c>
+      <c r="T46" s="27">
+        <v>1</v>
+      </c>
+      <c r="U46" s="27">
+        <v>0</v>
+      </c>
+      <c r="V46" s="27">
+        <v>0</v>
+      </c>
+      <c r="X46" s="27"/>
+      <c r="Y46" s="27"/>
+      <c r="Z46" s="27"/>
+      <c r="AA46" s="27">
+        <v>1</v>
+      </c>
+      <c r="AE46" s="26"/>
+      <c r="AF46" s="26"/>
+      <c r="AG46" s="26"/>
+      <c r="AH46" s="26"/>
+      <c r="AI46" s="26"/>
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A47" s="29">
+        <v>45</v>
+      </c>
+      <c r="B47" s="29">
+        <v>1</v>
+      </c>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29">
+        <v>1</v>
+      </c>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29">
+        <v>1</v>
+      </c>
+      <c r="J47" s="29">
+        <v>1</v>
+      </c>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="P47" s="27">
+        <v>45</v>
+      </c>
+      <c r="Q47" s="27">
+        <v>1</v>
+      </c>
+      <c r="R47" s="27">
+        <v>1</v>
+      </c>
+      <c r="S47" s="27">
+        <v>1</v>
+      </c>
+      <c r="T47" s="27">
+        <v>1</v>
+      </c>
+      <c r="U47" s="27">
+        <v>0</v>
+      </c>
+      <c r="V47" s="27">
+        <v>0</v>
+      </c>
+      <c r="X47" s="27"/>
+      <c r="Y47" s="27"/>
+      <c r="Z47" s="27"/>
+      <c r="AA47" s="27">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE47" s="26"/>
+      <c r="AF47" s="26"/>
+      <c r="AG47" s="26"/>
+      <c r="AH47" s="26"/>
+      <c r="AI47" s="26"/>
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A48" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="29">
+        <f>SUM(B3:B47)</f>
+        <v>45</v>
+      </c>
+      <c r="C48" s="29">
+        <f t="shared" ref="C48:N48" si="0">SUM(C3:C47)</f>
+        <v>24</v>
+      </c>
+      <c r="D48" s="29">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="E48" s="29">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F48" s="29">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="G48" s="29">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H48" s="29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I48" s="29">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="J48" s="29">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K48" s="29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L48" s="29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M48" s="29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="N48" s="29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="X48" s="27">
+        <f>SUM(X3:X47)</f>
+        <v>4</v>
+      </c>
+      <c r="Y48" s="27">
+        <f t="shared" ref="Y48:AA48" si="1">SUM(Y3:Y47)</f>
+        <v>11</v>
+      </c>
+      <c r="Z48" s="27">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AA48" s="27">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="AB48" s="27">
+        <f>SUM(X48:AA48)</f>
+        <v>44</v>
+      </c>
+      <c r="AE48" s="26"/>
+      <c r="AF48" s="26"/>
+      <c r="AG48" s="26"/>
+      <c r="AH48" s="26"/>
+      <c r="AI48" s="26"/>
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="A49" s="28"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="28"/>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="28"/>
+      <c r="X49" s="4"/>
+      <c r="Y49" s="4"/>
+      <c r="Z49" s="4"/>
+      <c r="AA49" s="4"/>
+      <c r="AE49" s="26"/>
+      <c r="AF49" s="26"/>
+      <c r="AG49" s="26"/>
+      <c r="AH49" s="26"/>
+      <c r="AI49" s="26"/>
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="X50" s="4"/>
+      <c r="Y50" s="4"/>
+      <c r="Z50" s="4"/>
+      <c r="AA50" s="4"/>
+      <c r="AE50" s="26"/>
+      <c r="AF50" s="26"/>
+      <c r="AG50" s="26"/>
+      <c r="AH50" s="26"/>
+      <c r="AI50" s="26"/>
+    </row>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="X51" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y51" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z51" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA51" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE51" s="26"/>
+      <c r="AF51" s="26"/>
+      <c r="AG51" s="26"/>
+      <c r="AH51" s="26"/>
+      <c r="AI51" s="26"/>
+    </row>
+    <row r="52" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="X52" s="34">
+        <f>X48/$AB$48</f>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="Y52" s="34">
+        <f t="shared" ref="Y52:AA52" si="2">Y48/$AB$48</f>
+        <v>0.25</v>
+      </c>
+      <c r="Z52" s="34">
+        <f t="shared" si="2"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="AA52" s="34">
+        <f t="shared" si="2"/>
+        <v>0.29545454545454547</v>
+      </c>
+      <c r="AE52" s="26"/>
+      <c r="AF52" s="26"/>
+      <c r="AG52" s="26"/>
+      <c r="AH52" s="26"/>
+      <c r="AI52" s="26"/>
+    </row>
+    <row r="53" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE53" s="26"/>
+      <c r="AF53" s="26"/>
+      <c r="AG53" s="26"/>
+      <c r="AH53" s="26"/>
+      <c r="AI53" s="26"/>
+    </row>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE54" s="26"/>
+      <c r="AF54" s="26"/>
+      <c r="AG54" s="26"/>
+      <c r="AH54" s="26"/>
+      <c r="AI54" s="26"/>
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE55" s="26"/>
+      <c r="AF55" s="26"/>
+      <c r="AG55" s="26"/>
+      <c r="AH55" s="26"/>
+      <c r="AI55" s="26"/>
+    </row>
+    <row r="56" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE56" s="26"/>
+      <c r="AF56" s="26"/>
+      <c r="AG56" s="26"/>
+      <c r="AH56" s="26"/>
+      <c r="AI56" s="26"/>
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE57" s="26"/>
+      <c r="AF57" s="26"/>
+      <c r="AG57" s="26"/>
+      <c r="AH57" s="26"/>
+      <c r="AI57" s="26"/>
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE58" s="26"/>
+      <c r="AF58" s="26"/>
+      <c r="AG58" s="26"/>
+      <c r="AH58" s="26"/>
+      <c r="AI58" s="26"/>
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE59" s="26"/>
+      <c r="AF59" s="26"/>
+      <c r="AG59" s="26"/>
+      <c r="AH59" s="26"/>
+      <c r="AI59" s="26"/>
+    </row>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE60" s="26"/>
+      <c r="AF60" s="26"/>
+      <c r="AG60" s="26"/>
+      <c r="AH60" s="26"/>
+      <c r="AI60" s="26"/>
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE61" s="26"/>
+      <c r="AF61" s="26"/>
+      <c r="AG61" s="26"/>
+      <c r="AH61" s="26"/>
+      <c r="AI61" s="26"/>
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE62" s="26"/>
+      <c r="AF62" s="26"/>
+      <c r="AG62" s="26"/>
+      <c r="AH62" s="26"/>
+      <c r="AI62" s="26"/>
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE63" s="26"/>
+      <c r="AF63" s="26"/>
+      <c r="AG63" s="26"/>
+      <c r="AH63" s="26"/>
+      <c r="AI63" s="26"/>
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="AE64" s="26"/>
+      <c r="AF64" s="26"/>
+      <c r="AG64" s="26"/>
+      <c r="AH64" s="26"/>
+      <c r="AI64" s="26"/>
+    </row>
+    <row r="65" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE65" s="26"/>
+      <c r="AF65" s="26"/>
+      <c r="AG65" s="26"/>
+      <c r="AH65" s="26"/>
+      <c r="AI65" s="26"/>
+    </row>
+    <row r="66" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE66" s="26"/>
+      <c r="AF66" s="26"/>
+      <c r="AG66" s="26"/>
+      <c r="AH66" s="26"/>
+      <c r="AI66" s="26"/>
+    </row>
+    <row r="67" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE67" s="26"/>
+      <c r="AF67" s="26"/>
+      <c r="AG67" s="26"/>
+      <c r="AH67" s="26"/>
+      <c r="AI67" s="26"/>
+    </row>
+    <row r="68" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE68" s="26"/>
+      <c r="AF68" s="26"/>
+      <c r="AG68" s="26"/>
+      <c r="AH68" s="26"/>
+      <c r="AI68" s="26"/>
+    </row>
+    <row r="69" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE69" s="26"/>
+      <c r="AF69" s="26"/>
+      <c r="AG69" s="26"/>
+      <c r="AH69" s="26"/>
+      <c r="AI69" s="26"/>
+    </row>
+    <row r="70" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE70" s="26"/>
+      <c r="AF70" s="26"/>
+      <c r="AG70" s="26"/>
+      <c r="AH70" s="26"/>
+      <c r="AI70" s="26"/>
+    </row>
+    <row r="71" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE71" s="26"/>
+      <c r="AF71" s="26"/>
+      <c r="AG71" s="26"/>
+      <c r="AH71" s="26"/>
+      <c r="AI71" s="26"/>
+    </row>
+    <row r="72" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE72" s="26"/>
+      <c r="AF72" s="26"/>
+      <c r="AG72" s="26"/>
+      <c r="AH72" s="26"/>
+      <c r="AI72" s="26"/>
+    </row>
+    <row r="73" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE73" s="26"/>
+      <c r="AF73" s="26"/>
+      <c r="AG73" s="26"/>
+      <c r="AH73" s="26"/>
+      <c r="AI73" s="26"/>
+    </row>
+    <row r="74" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE74" s="26"/>
+      <c r="AF74" s="26"/>
+      <c r="AG74" s="26"/>
+      <c r="AH74" s="26"/>
+      <c r="AI74" s="26"/>
+    </row>
+    <row r="75" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE75" s="26"/>
+      <c r="AF75" s="26"/>
+      <c r="AG75" s="26"/>
+      <c r="AH75" s="26"/>
+      <c r="AI75" s="26"/>
+    </row>
+    <row r="76" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE76" s="26"/>
+      <c r="AF76" s="26"/>
+      <c r="AG76" s="26"/>
+      <c r="AH76" s="26"/>
+      <c r="AI76" s="26"/>
+    </row>
+    <row r="77" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE77" s="26"/>
+      <c r="AF77" s="26"/>
+      <c r="AG77" s="26"/>
+      <c r="AH77" s="26"/>
+      <c r="AI77" s="26"/>
+    </row>
+    <row r="78" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE78" s="26"/>
+      <c r="AF78" s="26"/>
+      <c r="AG78" s="26"/>
+      <c r="AH78" s="26"/>
+      <c r="AI78" s="26"/>
+    </row>
+    <row r="79" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE79" s="26"/>
+      <c r="AF79" s="26"/>
+      <c r="AG79" s="26"/>
+      <c r="AH79" s="26"/>
+      <c r="AI79" s="26"/>
+    </row>
+    <row r="80" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE80" s="26"/>
+      <c r="AF80" s="26"/>
+      <c r="AG80" s="26"/>
+      <c r="AH80" s="26"/>
+      <c r="AI80" s="26"/>
+    </row>
+    <row r="81" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE81" s="26"/>
+      <c r="AF81" s="26"/>
+      <c r="AG81" s="26"/>
+      <c r="AH81" s="26"/>
+      <c r="AI81" s="26"/>
+    </row>
+    <row r="82" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE82" s="26"/>
+      <c r="AF82" s="26"/>
+      <c r="AH82" s="26"/>
+      <c r="AI82" s="26"/>
+    </row>
+    <row r="83" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE83" s="26"/>
+      <c r="AF83" s="26"/>
+      <c r="AH83" s="26"/>
+      <c r="AI83" s="26"/>
+    </row>
+    <row r="84" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE84" s="26"/>
+      <c r="AF84" s="26"/>
+      <c r="AH84" s="26"/>
+      <c r="AI84" s="26"/>
+    </row>
+    <row r="85" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE85" s="26"/>
+      <c r="AF85" s="26"/>
+      <c r="AH85" s="26"/>
+      <c r="AI85" s="26"/>
+    </row>
+    <row r="86" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AE86" s="26"/>
+      <c r="AF86" s="26"/>
+      <c r="AH86" s="26"/>
+      <c r="AI86" s="26"/>
+    </row>
+    <row r="87" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF87" s="26"/>
+      <c r="AH87" s="26"/>
+      <c r="AI87" s="26"/>
+    </row>
+    <row r="88" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF88" s="26"/>
+      <c r="AH88" s="26"/>
+      <c r="AI88" s="26"/>
+    </row>
+    <row r="89" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF89" s="26"/>
+      <c r="AH89" s="26"/>
+      <c r="AI89" s="26"/>
+    </row>
+    <row r="90" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF90" s="26"/>
+      <c r="AH90" s="26"/>
+      <c r="AI90" s="26"/>
+    </row>
+    <row r="91" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF91" s="26"/>
+      <c r="AH91" s="26"/>
+      <c r="AI91" s="26"/>
+    </row>
+    <row r="92" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF92" s="26"/>
+      <c r="AI92" s="26"/>
+    </row>
+    <row r="93" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF93" s="26"/>
+      <c r="AI93" s="26"/>
+    </row>
+    <row r="94" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AF94" s="26"/>
+      <c r="AI94" s="26"/>
+    </row>
+    <row r="95" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AI95" s="26"/>
+    </row>
+    <row r="96" spans="31:35" x14ac:dyDescent="0.2">
+      <c r="AI96" s="26"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="P1:V1"/>
+    <mergeCell ref="X1:AA1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>